<commit_message>
Edited Readme in dataset_main to correspond to the relative price series you defined
That’s all I changed. But I also looked through read_data2.m and it
looks great! There are only 2 things that may be a problem:
1.) We need transformations to account for cases where more than one
transformation happens, e.g. log and difference.
2) I’m not sure I understand exactly what’s going on with the
“generalized truncation”.
</commit_message>
<xml_diff>
--- a/Data/dataset_main.xlsx
+++ b/Data/dataset_main.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\th3\Documents\BG_2017\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="0" windowWidth="25605" windowHeight="15465" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="333">
   <si>
     <t>Name</t>
   </si>
@@ -1021,12 +1016,15 @@
   </si>
   <si>
     <t>Rel_Price</t>
+  </si>
+  <si>
+    <t>just = P_IT / CPI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1640,28 +1638,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="16.625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="16.625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="16.625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="16.625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="16.625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="16.625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="16.625" style="9" customWidth="1"/>
-    <col min="12" max="12" width="12.875" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="10.875" style="9"/>
+    <col min="1" max="1" width="14.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1698,8 +1696,11 @@
       <c r="L1" s="3" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="195">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -1787,7 +1788,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="31.5">
       <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
@@ -1822,7 +1823,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="63">
       <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="78.75">
       <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="2" customFormat="1">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
@@ -1921,7 +1922,7 @@
         <v>43056</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="135">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -1933,6 +1934,9 @@
       <c r="H8" s="3"/>
       <c r="J8" s="3"/>
       <c r="L8" s="3"/>
+      <c r="M8" s="2" t="s">
+        <v>332</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1949,19 +1953,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="23.375" style="13"/>
+    <col min="5" max="5" width="23.33203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="23.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2002,7 +2006,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="21">
       <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
@@ -2043,7 +2047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="21">
       <c r="A3" s="20" t="s">
         <v>330</v>
       </c>
@@ -2084,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="21">
       <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
@@ -2125,7 +2129,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="21">
       <c r="A5" s="24" t="s">
         <v>24</v>
       </c>
@@ -2165,7 +2169,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="21">
       <c r="A6" s="24" t="s">
         <v>25</v>
       </c>
@@ -2207,7 +2211,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="21">
       <c r="A7" s="24" t="s">
         <v>26</v>
       </c>
@@ -2249,7 +2253,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="21">
       <c r="A8" s="24" t="s">
         <v>27</v>
       </c>
@@ -2291,7 +2295,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="21">
       <c r="A9" s="24" t="s">
         <v>28</v>
       </c>
@@ -2333,7 +2337,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="21">
       <c r="A10" s="24" t="s">
         <v>29</v>
       </c>
@@ -2375,7 +2379,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="21">
       <c r="A11" s="24" t="s">
         <v>30</v>
       </c>
@@ -2417,7 +2421,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="21">
       <c r="A12" s="24" t="s">
         <v>31</v>
       </c>
@@ -2459,7 +2463,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="21">
       <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
@@ -2501,7 +2505,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="21">
       <c r="A14" s="24" t="s">
         <v>33</v>
       </c>
@@ -2543,7 +2547,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="21">
       <c r="A15" s="24" t="s">
         <v>34</v>
       </c>
@@ -2585,7 +2589,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="21">
       <c r="A16" s="24" t="s">
         <v>35</v>
       </c>
@@ -2627,7 +2631,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="21">
       <c r="A17" s="24" t="s">
         <v>36</v>
       </c>
@@ -2669,7 +2673,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="21">
       <c r="A18" s="24" t="s">
         <v>37</v>
       </c>
@@ -2711,7 +2715,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="21">
       <c r="A19" s="24" t="s">
         <v>38</v>
       </c>
@@ -2753,7 +2757,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="21">
       <c r="A20" s="24" t="s">
         <v>39</v>
       </c>
@@ -2795,7 +2799,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="21">
       <c r="A21" s="24" t="s">
         <v>40</v>
       </c>
@@ -2837,7 +2841,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="21">
       <c r="A22" s="24" t="s">
         <v>41</v>
       </c>
@@ -2879,7 +2883,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="21">
       <c r="A23" s="24" t="s">
         <v>42</v>
       </c>
@@ -2921,7 +2925,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="21">
       <c r="A24" s="24" t="s">
         <v>43</v>
       </c>
@@ -2963,7 +2967,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="21">
       <c r="A25" s="24" t="s">
         <v>44</v>
       </c>
@@ -3005,7 +3009,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="21">
       <c r="A26" s="24" t="s">
         <v>45</v>
       </c>
@@ -3047,7 +3051,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="21">
       <c r="A27" s="24" t="s">
         <v>46</v>
       </c>
@@ -3089,7 +3093,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="21">
       <c r="A28" s="24" t="s">
         <v>47</v>
       </c>
@@ -3131,7 +3135,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="21">
       <c r="A29" s="24" t="s">
         <v>48</v>
       </c>
@@ -3173,7 +3177,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="21">
       <c r="A30" s="24" t="s">
         <v>49</v>
       </c>
@@ -3215,7 +3219,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="21">
       <c r="A31" s="24" t="s">
         <v>50</v>
       </c>
@@ -3257,7 +3261,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="21">
       <c r="A32" s="24" t="s">
         <v>51</v>
       </c>
@@ -3299,7 +3303,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" ht="21">
       <c r="A33" s="24" t="s">
         <v>52</v>
       </c>
@@ -3341,7 +3345,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" ht="21">
       <c r="A34" s="24" t="s">
         <v>53</v>
       </c>
@@ -3383,7 +3387,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" ht="21">
       <c r="A35" s="24" t="s">
         <v>54</v>
       </c>
@@ -3425,7 +3429,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" ht="21">
       <c r="A36" s="24" t="s">
         <v>55</v>
       </c>
@@ -3467,7 +3471,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" ht="21">
       <c r="A37" s="24" t="s">
         <v>56</v>
       </c>
@@ -3509,7 +3513,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" ht="21">
       <c r="A38" s="24" t="s">
         <v>57</v>
       </c>
@@ -3551,7 +3555,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" ht="21">
       <c r="A39" s="24" t="s">
         <v>58</v>
       </c>
@@ -3593,7 +3597,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" ht="21">
       <c r="A40" s="24" t="s">
         <v>59</v>
       </c>
@@ -3635,7 +3639,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="21">
       <c r="A41" s="24" t="s">
         <v>60</v>
       </c>
@@ -3677,7 +3681,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" ht="21">
       <c r="A42" s="24" t="s">
         <v>61</v>
       </c>
@@ -3719,7 +3723,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="21">
       <c r="A43" s="24" t="s">
         <v>62</v>
       </c>
@@ -3761,7 +3765,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="21">
       <c r="A44" s="24" t="s">
         <v>63</v>
       </c>
@@ -3803,7 +3807,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" ht="21">
       <c r="A45" s="24" t="s">
         <v>64</v>
       </c>
@@ -3845,7 +3849,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" ht="21">
       <c r="A46" s="24" t="s">
         <v>65</v>
       </c>
@@ -3887,7 +3891,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="21">
       <c r="A47" s="24" t="s">
         <v>66</v>
       </c>
@@ -3929,7 +3933,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="21">
       <c r="A48" s="24" t="s">
         <v>67</v>
       </c>
@@ -3971,7 +3975,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="21">
       <c r="A49" s="24" t="s">
         <v>68</v>
       </c>
@@ -4013,7 +4017,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" ht="21">
       <c r="A50" s="24" t="s">
         <v>69</v>
       </c>
@@ -4055,7 +4059,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" ht="21">
       <c r="A51" s="24" t="s">
         <v>70</v>
       </c>
@@ -4097,7 +4101,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" ht="21">
       <c r="A52" s="24" t="s">
         <v>71</v>
       </c>
@@ -4139,7 +4143,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" ht="21">
       <c r="A53" s="24" t="s">
         <v>72</v>
       </c>
@@ -4181,7 +4185,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" ht="21">
       <c r="A54" s="24" t="s">
         <v>73</v>
       </c>
@@ -4223,7 +4227,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="21">
       <c r="A55" s="24" t="s">
         <v>74</v>
       </c>
@@ -4265,7 +4269,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" ht="21">
       <c r="A56" s="24" t="s">
         <v>75</v>
       </c>
@@ -4307,7 +4311,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" ht="21">
       <c r="A57" s="24" t="s">
         <v>76</v>
       </c>
@@ -4349,7 +4353,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" ht="21">
       <c r="A58" s="24" t="s">
         <v>77</v>
       </c>
@@ -4391,7 +4395,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" ht="21">
       <c r="A59" s="24" t="s">
         <v>78</v>
       </c>
@@ -4433,7 +4437,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" ht="21">
       <c r="A60" s="24" t="s">
         <v>79</v>
       </c>
@@ -4475,7 +4479,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" ht="21">
       <c r="A61" s="24" t="s">
         <v>80</v>
       </c>
@@ -4517,7 +4521,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" ht="21">
       <c r="A62" s="24" t="s">
         <v>81</v>
       </c>
@@ -4559,7 +4563,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" ht="21">
       <c r="A63" s="24" t="s">
         <v>82</v>
       </c>
@@ -4601,7 +4605,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" ht="21">
       <c r="A64" s="24" t="s">
         <v>83</v>
       </c>
@@ -4643,7 +4647,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" ht="21">
       <c r="A65" s="24" t="s">
         <v>84</v>
       </c>
@@ -4685,7 +4689,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" ht="21">
       <c r="A66" s="24" t="s">
         <v>85</v>
       </c>
@@ -4727,7 +4731,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" ht="21">
       <c r="A67" s="24" t="s">
         <v>86</v>
       </c>
@@ -4769,7 +4773,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" ht="21">
       <c r="A68" s="24" t="s">
         <v>87</v>
       </c>
@@ -4811,7 +4815,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" ht="21">
       <c r="A69" s="24" t="s">
         <v>88</v>
       </c>
@@ -4853,7 +4857,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" ht="21">
       <c r="A70" s="24" t="s">
         <v>89</v>
       </c>
@@ -4895,7 +4899,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" ht="21">
       <c r="A71" s="24" t="s">
         <v>90</v>
       </c>
@@ -4937,7 +4941,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" ht="21">
       <c r="A72" s="24" t="s">
         <v>91</v>
       </c>
@@ -4979,7 +4983,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" ht="21">
       <c r="A73" s="24" t="s">
         <v>92</v>
       </c>
@@ -5021,7 +5025,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" ht="21">
       <c r="A74" s="24" t="s">
         <v>93</v>
       </c>
@@ -5063,7 +5067,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" ht="21">
       <c r="A75" s="24" t="s">
         <v>94</v>
       </c>
@@ -5105,7 +5109,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" ht="21">
       <c r="A76" s="24" t="s">
         <v>95</v>
       </c>
@@ -5147,7 +5151,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" ht="21">
       <c r="A77" s="24" t="s">
         <v>96</v>
       </c>
@@ -5189,7 +5193,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" ht="21">
       <c r="A78" s="24" t="s">
         <v>97</v>
       </c>
@@ -5231,7 +5235,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" ht="21">
       <c r="A79" s="24" t="s">
         <v>98</v>
       </c>
@@ -5273,7 +5277,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" ht="21">
       <c r="A80" s="24" t="s">
         <v>99</v>
       </c>
@@ -5315,7 +5319,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" ht="21">
       <c r="A81" s="24" t="s">
         <v>100</v>
       </c>
@@ -5357,7 +5361,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" ht="21">
       <c r="A82" s="24" t="s">
         <v>101</v>
       </c>
@@ -5399,7 +5403,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" ht="21">
       <c r="A83" s="24" t="s">
         <v>102</v>
       </c>
@@ -5441,7 +5445,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" ht="21">
       <c r="A84" s="24" t="s">
         <v>103</v>
       </c>
@@ -5483,7 +5487,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" ht="21">
       <c r="A85" s="24" t="s">
         <v>104</v>
       </c>
@@ -5525,7 +5529,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" ht="21">
       <c r="A86" s="24" t="s">
         <v>105</v>
       </c>
@@ -5567,7 +5571,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" ht="21">
       <c r="A87" s="24" t="s">
         <v>106</v>
       </c>
@@ -5609,7 +5613,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" ht="21">
       <c r="A88" s="24" t="s">
         <v>107</v>
       </c>
@@ -5651,7 +5655,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" ht="21">
       <c r="A89" s="24" t="s">
         <v>108</v>
       </c>
@@ -5693,7 +5697,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" ht="21">
       <c r="A90" s="24" t="s">
         <v>109</v>
       </c>
@@ -5735,7 +5739,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" ht="21">
       <c r="A91" s="24" t="s">
         <v>110</v>
       </c>
@@ -5777,7 +5781,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" ht="21">
       <c r="A92" s="24" t="s">
         <v>111</v>
       </c>
@@ -5819,7 +5823,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" ht="21">
       <c r="A93" s="24" t="s">
         <v>113</v>
       </c>
@@ -5861,7 +5865,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" ht="21">
       <c r="A94" s="24" t="s">
         <v>114</v>
       </c>
@@ -5903,7 +5907,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" ht="21">
       <c r="A95" s="24" t="s">
         <v>115</v>
       </c>
@@ -5945,7 +5949,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" ht="21">
       <c r="A96" s="24" t="s">
         <v>116</v>
       </c>
@@ -5987,7 +5991,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" ht="21">
       <c r="A97" s="24" t="s">
         <v>117</v>
       </c>
@@ -6029,7 +6033,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" ht="21">
       <c r="A98" s="24" t="s">
         <v>118</v>
       </c>
@@ -6071,7 +6075,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" ht="21">
       <c r="A99" s="24" t="s">
         <v>119</v>
       </c>
@@ -6113,7 +6117,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" ht="21">
       <c r="A100" s="24" t="s">
         <v>120</v>
       </c>
@@ -6155,7 +6159,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" ht="21">
       <c r="A101" s="24" t="s">
         <v>121</v>
       </c>
@@ -6197,7 +6201,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" ht="21">
       <c r="A102" s="24" t="s">
         <v>122</v>
       </c>
@@ -6239,7 +6243,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" ht="21">
       <c r="A103" s="24" t="s">
         <v>123</v>
       </c>
@@ -6281,7 +6285,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" ht="21">
       <c r="A104" s="24" t="s">
         <v>124</v>
       </c>
@@ -6323,7 +6327,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" ht="21">
       <c r="A105" s="24" t="s">
         <v>125</v>
       </c>
@@ -6365,7 +6369,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" ht="21">
       <c r="A106" s="24" t="s">
         <v>126</v>
       </c>
@@ -6407,7 +6411,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" ht="21">
       <c r="A107" s="24" t="s">
         <v>127</v>
       </c>
@@ -6449,7 +6453,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" ht="21">
       <c r="A108" s="24" t="s">
         <v>128</v>
       </c>
@@ -6491,7 +6495,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" ht="21">
       <c r="A109" s="24" t="s">
         <v>129</v>
       </c>
@@ -6533,7 +6537,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" ht="21">
       <c r="A110" s="24" t="s">
         <v>130</v>
       </c>
@@ -6575,7 +6579,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" ht="21">
       <c r="A111" s="24" t="s">
         <v>131</v>
       </c>
@@ -6617,7 +6621,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" ht="21">
       <c r="A112" s="24" t="s">
         <v>132</v>
       </c>
@@ -6659,7 +6663,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" ht="21">
       <c r="A113" s="24" t="s">
         <v>133</v>
       </c>
@@ -6701,7 +6705,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" ht="21">
       <c r="A114" s="24" t="s">
         <v>134</v>
       </c>
@@ -6743,7 +6747,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" ht="21">
       <c r="A115" s="24" t="s">
         <v>135</v>
       </c>
@@ -6785,7 +6789,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" ht="21">
       <c r="A116" s="24" t="s">
         <v>136</v>
       </c>
@@ -6827,7 +6831,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" ht="21">
       <c r="A117" s="24" t="s">
         <v>137</v>
       </c>
@@ -6869,7 +6873,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:13" ht="21">
       <c r="A118" s="24" t="s">
         <v>138</v>
       </c>
@@ -6911,7 +6915,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" ht="21">
       <c r="A119" s="24" t="s">
         <v>139</v>
       </c>
@@ -6953,7 +6957,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" ht="21">
       <c r="A120" s="24" t="s">
         <v>140</v>
       </c>
@@ -6995,7 +6999,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:13" ht="21">
       <c r="A121" s="24" t="s">
         <v>141</v>
       </c>
@@ -7037,7 +7041,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:13" ht="21">
       <c r="A122" s="24" t="s">
         <v>142</v>
       </c>
@@ -7079,7 +7083,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:13" ht="21">
       <c r="A123" s="24" t="s">
         <v>143</v>
       </c>
@@ -7121,7 +7125,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:13" ht="21">
       <c r="A124" s="24" t="s">
         <v>144</v>
       </c>
@@ -7163,7 +7167,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:13" ht="21">
       <c r="A125" s="24" t="s">
         <v>145</v>
       </c>
@@ -7205,7 +7209,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:13" ht="21">
       <c r="A126" s="24" t="s">
         <v>146</v>
       </c>
@@ -7247,7 +7251,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:13" ht="21">
       <c r="A127" s="24" t="s">
         <v>147</v>
       </c>
@@ -7289,7 +7293,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:13" ht="21">
       <c r="A128" s="24" t="s">
         <v>148</v>
       </c>
@@ -7331,7 +7335,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" ht="21">
       <c r="A129" s="24" t="s">
         <v>149</v>
       </c>
@@ -7373,7 +7377,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" ht="21">
       <c r="A130" s="24" t="s">
         <v>150</v>
       </c>
@@ -7415,7 +7419,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" ht="21">
       <c r="A131" s="24" t="s">
         <v>151</v>
       </c>
@@ -7457,7 +7461,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" ht="21">
       <c r="A132" s="24" t="s">
         <v>152</v>
       </c>
@@ -7499,7 +7503,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" ht="21">
       <c r="A133" s="24" t="s">
         <v>153</v>
       </c>
@@ -7541,7 +7545,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:13" ht="21">
       <c r="A134" s="24" t="s">
         <v>154</v>
       </c>
@@ -7583,7 +7587,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" ht="21">
       <c r="A135" s="24" t="s">
         <v>155</v>
       </c>
@@ -7625,7 +7629,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" ht="21">
       <c r="A136" s="24" t="s">
         <v>156</v>
       </c>
@@ -7667,7 +7671,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:13" ht="21">
       <c r="A137" s="24" t="s">
         <v>157</v>
       </c>
@@ -7709,7 +7713,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="138" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:13" ht="21">
       <c r="A138" s="24" t="s">
         <v>158</v>
       </c>
@@ -7751,7 +7755,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="139" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:13" ht="21">
       <c r="A139" s="24" t="s">
         <v>159</v>
       </c>
@@ -7793,7 +7797,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="140" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:13" ht="21">
       <c r="A140" s="24" t="s">
         <v>160</v>
       </c>
@@ -7835,7 +7839,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="141" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" ht="21">
       <c r="A141" s="24" t="s">
         <v>161</v>
       </c>
@@ -7877,7 +7881,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" ht="21">
       <c r="A142" s="24" t="s">
         <v>162</v>
       </c>
@@ -7919,7 +7923,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" ht="21">
       <c r="A143" s="24" t="s">
         <v>163</v>
       </c>
@@ -7961,7 +7965,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" ht="21">
       <c r="A144" s="24" t="s">
         <v>164</v>
       </c>
@@ -8003,7 +8007,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" ht="21">
       <c r="A145" s="24" t="s">
         <v>165</v>
       </c>
@@ -8045,7 +8049,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" ht="21">
       <c r="A146" s="24" t="s">
         <v>166</v>
       </c>
@@ -8087,7 +8091,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" ht="21">
       <c r="A147" s="24" t="s">
         <v>167</v>
       </c>
@@ -8129,7 +8133,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" ht="21">
       <c r="A148" s="24" t="s">
         <v>168</v>
       </c>
@@ -8171,7 +8175,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" ht="21">
       <c r="A149" s="24" t="s">
         <v>169</v>
       </c>
@@ -8213,7 +8217,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" ht="21">
       <c r="A150" s="24" t="s">
         <v>170</v>
       </c>
@@ -8255,7 +8259,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" ht="21">
       <c r="A151" s="24" t="s">
         <v>171</v>
       </c>
@@ -8297,7 +8301,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" ht="21">
       <c r="A152" s="24" t="s">
         <v>172</v>
       </c>
@@ -8339,7 +8343,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" ht="21">
       <c r="A153" s="24" t="s">
         <v>173</v>
       </c>
@@ -8381,7 +8385,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" ht="21">
       <c r="A154" s="24" t="s">
         <v>174</v>
       </c>
@@ -8423,7 +8427,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" ht="21">
       <c r="A155" s="24" t="s">
         <v>175</v>
       </c>
@@ -8465,7 +8469,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" ht="21">
       <c r="A156" s="24" t="s">
         <v>176</v>
       </c>
@@ -8507,7 +8511,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" ht="21">
       <c r="A157" s="24" t="s">
         <v>177</v>
       </c>
@@ -8549,7 +8553,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" ht="21">
       <c r="A158" s="24" t="s">
         <v>178</v>
       </c>
@@ -8591,7 +8595,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" ht="21">
       <c r="A159" s="24" t="s">
         <v>179</v>
       </c>
@@ -8633,7 +8637,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" ht="21">
       <c r="A160" s="24" t="s">
         <v>180</v>
       </c>
@@ -8675,7 +8679,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="161" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" ht="21">
       <c r="A161" s="24" t="s">
         <v>181</v>
       </c>
@@ -8717,7 +8721,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" ht="21">
       <c r="A162" s="24" t="s">
         <v>182</v>
       </c>
@@ -8759,7 +8763,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" ht="21">
       <c r="A163" s="24" t="s">
         <v>183</v>
       </c>
@@ -8801,7 +8805,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" ht="21">
       <c r="A164" s="24" t="s">
         <v>184</v>
       </c>
@@ -8843,7 +8847,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" ht="21">
       <c r="A165" s="24" t="s">
         <v>185</v>
       </c>
@@ -8885,7 +8889,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" ht="21">
       <c r="A166" s="24" t="s">
         <v>186</v>
       </c>
@@ -8927,7 +8931,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" ht="21">
       <c r="A167" s="24" t="s">
         <v>187</v>
       </c>
@@ -8969,7 +8973,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" ht="21">
       <c r="A168" s="24" t="s">
         <v>188</v>
       </c>
@@ -9011,7 +9015,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" ht="21">
       <c r="A169" s="24" t="s">
         <v>189</v>
       </c>
@@ -9053,7 +9057,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" ht="21">
       <c r="A170" s="24" t="s">
         <v>190</v>
       </c>
@@ -9095,7 +9099,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="171" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" ht="21">
       <c r="A171" s="24" t="s">
         <v>191</v>
       </c>
@@ -9137,7 +9141,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" ht="21">
       <c r="A172" s="24" t="s">
         <v>192</v>
       </c>
@@ -9179,7 +9183,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" ht="21">
       <c r="A173" s="24" t="s">
         <v>193</v>
       </c>
@@ -9221,7 +9225,7 @@
         <v>0.8126022913256955</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" ht="21">
       <c r="A174" s="24" t="s">
         <v>194</v>
       </c>
@@ -9263,7 +9267,7 @@
         <v>0.77679290894439978</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" ht="21">
       <c r="A175" s="24" t="s">
         <v>195</v>
       </c>
@@ -9305,7 +9309,7 @@
         <v>0.7548076923076924</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" ht="21">
       <c r="A176" s="24" t="s">
         <v>196</v>
       </c>
@@ -9347,7 +9351,7 @@
         <v>0.73396674584323041</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" ht="21">
       <c r="A177" s="24" t="s">
         <v>197</v>
       </c>
@@ -9389,7 +9393,7 @@
         <v>0.73017107309486784</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" ht="21">
       <c r="A178" s="24" t="s">
         <v>198</v>
       </c>
@@ -9431,7 +9435,7 @@
         <v>0.72671285604311009</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" ht="21">
       <c r="A179" s="24" t="s">
         <v>199</v>
       </c>
@@ -9473,7 +9477,7 @@
         <v>0.71849056603773587</v>
       </c>
     </row>
-    <row r="180" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" ht="21">
       <c r="A180" s="24" t="s">
         <v>200</v>
       </c>
@@ -9515,7 +9519,7 @@
         <v>0.67287630402384502</v>
       </c>
     </row>
-    <row r="181" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" ht="21">
       <c r="A181" s="24" t="s">
         <v>201</v>
       </c>
@@ -9557,7 +9561,7 @@
         <v>0.67062314540059342</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" ht="21">
       <c r="A182" s="24" t="s">
         <v>202</v>
       </c>
@@ -9599,7 +9603,7 @@
         <v>0.65294117647058825</v>
       </c>
     </row>
-    <row r="183" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" ht="21">
       <c r="A183" s="24" t="s">
         <v>203</v>
       </c>
@@ -9641,7 +9645,7 @@
         <v>0.63795620437956213</v>
       </c>
     </row>
-    <row r="184" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" ht="21">
       <c r="A184" s="24" t="s">
         <v>204</v>
       </c>
@@ -9683,7 +9687,7 @@
         <v>0.62662807525325614</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" ht="21">
       <c r="A185" s="24" t="s">
         <v>205</v>
       </c>
@@ -9725,7 +9729,7 @@
         <v>0.61897915168943207</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" ht="21">
       <c r="A186" s="24" t="s">
         <v>206</v>
       </c>
@@ -9767,7 +9771,7 @@
         <v>0.59743040685224846</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" ht="21">
       <c r="A187" s="24" t="s">
         <v>207</v>
       </c>
@@ -9809,7 +9813,7 @@
         <v>0.58823529411764708</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:13" ht="21">
       <c r="A188" s="24" t="s">
         <v>208</v>
       </c>
@@ -9851,7 +9855,7 @@
         <v>0.57132817990161622</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:13" ht="21">
       <c r="A189" s="24" t="s">
         <v>209</v>
       </c>
@@ -9893,7 +9897,7 @@
         <v>0.56454989532449407</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:13" ht="21">
       <c r="A190" s="24" t="s">
         <v>210</v>
       </c>
@@ -9935,7 +9939,7 @@
         <v>0.55301455301455293</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:13" ht="21">
       <c r="A191" s="24" t="s">
         <v>211</v>
       </c>
@@ -9977,7 +9981,7 @@
         <v>0.53448275862068961</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:13" ht="21">
       <c r="A192" s="24" t="s">
         <v>212</v>
       </c>
@@ -10019,7 +10023,7 @@
         <v>0.51332877648667119</v>
       </c>
     </row>
-    <row r="193" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:13" ht="21">
       <c r="A193" s="24" t="s">
         <v>213</v>
       </c>
@@ -10061,7 +10065,7 @@
         <v>0.50033990482664847</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:13" ht="21">
       <c r="A194" s="24" t="s">
         <v>214</v>
       </c>
@@ -10103,7 +10107,7 @@
         <v>0.49290060851926981</v>
       </c>
     </row>
-    <row r="195" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:13" ht="21">
       <c r="A195" s="24" t="s">
         <v>215</v>
       </c>
@@ -10145,7 +10149,7 @@
         <v>0.4688546550569323</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:13" ht="21">
       <c r="A196" s="24" t="s">
         <v>216</v>
       </c>
@@ -10187,7 +10191,7 @@
         <v>0.45502998001332445</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:13" ht="21">
       <c r="A197" s="24" t="s">
         <v>217</v>
       </c>
@@ -10229,7 +10233,7 @@
         <v>0.42460317460317465</v>
       </c>
     </row>
-    <row r="198" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:13" ht="21">
       <c r="A198" s="24" t="s">
         <v>218</v>
       </c>
@@ -10271,7 +10275,7 @@
         <v>0.42388451443569547</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:13" ht="21">
       <c r="A199" s="24" t="s">
         <v>219</v>
       </c>
@@ -10313,7 +10317,7 @@
         <v>0.41476159372958854</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:13" ht="21">
       <c r="A200" s="24" t="s">
         <v>220</v>
       </c>
@@ -10355,7 +10359,7 @@
         <v>0.39636127355425599</v>
       </c>
     </row>
-    <row r="201" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:13" ht="21">
       <c r="A201" s="24" t="s">
         <v>221</v>
       </c>
@@ -10397,7 +10401,7 @@
         <v>0.38842443729903536</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:13" ht="21">
       <c r="A202" s="24" t="s">
         <v>222</v>
       </c>
@@ -10439,7 +10443,7 @@
         <v>0.37141033822590941</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:13" ht="21">
       <c r="A203" s="24" t="s">
         <v>223</v>
       </c>
@@ -10481,7 +10485,7 @@
         <v>0.35066582117945466</v>
       </c>
     </row>
-    <row r="204" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:13" ht="21">
       <c r="A204" s="24" t="s">
         <v>224</v>
       </c>
@@ -10523,7 +10527,7 @@
         <v>0.33878064110622252</v>
       </c>
     </row>
-    <row r="205" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:13" ht="21">
       <c r="A205" s="24" t="s">
         <v>225</v>
       </c>
@@ -10565,7 +10569,7 @@
         <v>0.32790988735919896</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:13" ht="21">
       <c r="A206" s="24" t="s">
         <v>226</v>
       </c>
@@ -10607,7 +10611,7 @@
         <v>0.31148564294631714</v>
       </c>
     </row>
-    <row r="207" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:13" ht="21">
       <c r="A207" s="24" t="s">
         <v>227</v>
       </c>
@@ -10649,7 +10653,7 @@
         <v>0.30086848635235736</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:13" ht="21">
       <c r="A208" s="24" t="s">
         <v>228</v>
       </c>
@@ -10691,7 +10695,7 @@
         <v>0.29295426452410378</v>
       </c>
     </row>
-    <row r="209" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:13" ht="21">
       <c r="A209" s="24" t="s">
         <v>229</v>
       </c>
@@ -10733,7 +10737,7 @@
         <v>0.26790123456790121</v>
       </c>
     </row>
-    <row r="210" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:13" ht="21">
       <c r="A210" s="24" t="s">
         <v>230</v>
       </c>
@@ -10775,7 +10779,7 @@
         <v>0.24938574938574937</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:13" ht="21">
       <c r="A211" s="24" t="s">
         <v>231</v>
       </c>
@@ -10817,7 +10821,7 @@
         <v>0.22446483180428137</v>
       </c>
     </row>
-    <row r="212" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:13" ht="21">
       <c r="A212" s="24" t="s">
         <v>232</v>
       </c>
@@ -10859,7 +10863,7 @@
         <v>0.21167883211678828</v>
       </c>
     </row>
-    <row r="213" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:13" ht="21">
       <c r="A213" s="24" t="s">
         <v>233</v>
       </c>
@@ -10901,7 +10905,7 @@
         <v>0.19660194174757278</v>
       </c>
     </row>
-    <row r="214" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:13" ht="21">
       <c r="A214" s="24" t="s">
         <v>234</v>
       </c>
@@ -10943,7 +10947,7 @@
         <v>0.17951807228915664</v>
       </c>
     </row>
-    <row r="215" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:13" ht="21">
       <c r="A215" s="24" t="s">
         <v>235</v>
       </c>
@@ -10985,7 +10989,7 @@
         <v>0.17461263408820024</v>
       </c>
     </row>
-    <row r="216" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:13" ht="21">
       <c r="A216" s="24" t="s">
         <v>236</v>
       </c>
@@ -11027,7 +11031,7 @@
         <v>0.16706161137440756</v>
       </c>
     </row>
-    <row r="217" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:13" ht="21">
       <c r="A217" s="24" t="s">
         <v>237</v>
       </c>
@@ -11069,7 +11073,7 @@
         <v>0.1590643274853801</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:13" ht="21">
       <c r="A218" s="24" t="s">
         <v>238</v>
       </c>
@@ -11111,7 +11115,7 @@
         <v>0.15098722415795587</v>
       </c>
     </row>
-    <row r="219" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:13" ht="21">
       <c r="A219" s="24" t="s">
         <v>239</v>
       </c>
@@ -11153,7 +11157,7 @@
         <v>0.14400921658986177</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:13" ht="21">
       <c r="A220" s="24" t="s">
         <v>240</v>
       </c>
@@ -11195,7 +11199,7 @@
         <v>0.13631156930126004</v>
       </c>
     </row>
-    <row r="221" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:13" ht="21">
       <c r="A221" s="24" t="s">
         <v>241</v>
       </c>
@@ -11237,7 +11241,7 @@
         <v>0.12776831345826237</v>
       </c>
     </row>
-    <row r="222" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:13" ht="21">
       <c r="A222" s="24" t="s">
         <v>242</v>
       </c>
@@ -11279,7 +11283,7 @@
         <v>0.12042768711311198</v>
       </c>
     </row>
-    <row r="223" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:13" ht="21">
       <c r="A223" s="24" t="s">
         <v>243</v>
       </c>
@@ -11321,7 +11325,7 @@
         <v>0.11398090960134756</v>
       </c>
     </row>
-    <row r="224" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:13" ht="21">
       <c r="A224" s="24" t="s">
         <v>244</v>
       </c>
@@ -11363,7 +11367,7 @@
         <v>0.11161217587373168</v>
       </c>
     </row>
-    <row r="225" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:13" ht="21">
       <c r="A225" s="24" t="s">
         <v>245</v>
       </c>
@@ -11405,7 +11409,7 @@
         <v>0.10532212885154062</v>
       </c>
     </row>
-    <row r="226" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:13" ht="21">
       <c r="A226" s="24" t="s">
         <v>246</v>
       </c>
@@ -11447,7 +11451,7 @@
         <v>0.10244988864142539</v>
       </c>
     </row>
-    <row r="227" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:13" ht="21">
       <c r="A227" s="24" t="s">
         <v>247</v>
       </c>
@@ -11489,7 +11493,7 @@
         <v>9.8451327433628319E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:13" ht="21">
       <c r="A228" s="24" t="s">
         <v>248</v>
       </c>
@@ -11531,7 +11535,7 @@
         <v>9.4609460946094598E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:13" ht="21">
       <c r="A229" s="24" t="s">
         <v>249</v>
       </c>
@@ -11573,7 +11577,7 @@
         <v>9.1353996737357265E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:13" ht="21">
       <c r="A230" s="24" t="s">
         <v>250</v>
       </c>
@@ -11615,7 +11619,7 @@
         <v>8.8476242490442378E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:13" ht="21">
       <c r="A231" s="24" t="s">
         <v>251</v>
       </c>
@@ -11657,7 +11661,7 @@
         <v>8.4278768233387355E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:13" ht="21">
       <c r="A232" s="24" t="s">
         <v>252</v>
       </c>
@@ -11699,7 +11703,7 @@
         <v>8.2479784366576825E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:13" ht="21">
       <c r="A233" s="24" t="s">
         <v>253</v>
       </c>
@@ -11741,7 +11745,7 @@
         <v>8.1239978621058251E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:13" ht="21">
       <c r="A234" s="24" t="s">
         <v>254</v>
       </c>
@@ -11783,7 +11787,7 @@
         <v>7.8877713075701433E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:13" ht="21">
       <c r="A235" s="24" t="s">
         <v>255</v>
       </c>
@@ -11825,7 +11829,7 @@
         <v>7.7449947312961009E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:13" ht="21">
       <c r="A236" s="24" t="s">
         <v>256</v>
       </c>
@@ -11867,7 +11871,7 @@
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:13" ht="21">
       <c r="A237" s="24" t="s">
         <v>257</v>
       </c>
@@ -11909,7 +11913,7 @@
         <v>7.2501294665976185E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:13" ht="21">
       <c r="A238" s="24" t="s">
         <v>258</v>
       </c>
@@ -11951,7 +11955,7 @@
         <v>7.0211667527103769E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:13" ht="21">
       <c r="A239" s="24" t="s">
         <v>259</v>
       </c>
@@ -11993,7 +11997,7 @@
         <v>6.6901408450704219E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:13" ht="21">
       <c r="A240" s="24" t="s">
         <v>260</v>
       </c>
@@ -12035,7 +12039,7 @@
         <v>6.6128218071680969E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:13" ht="21">
       <c r="A241" s="24" t="s">
         <v>261</v>
       </c>
@@ -12077,7 +12081,7 @@
         <v>6.5097646469704562E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:13" ht="21">
       <c r="A242" s="24" t="s">
         <v>262</v>
       </c>
@@ -12119,7 +12123,7 @@
         <v>6.2933597621407322E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:13" ht="21">
       <c r="A243" s="24" t="s">
         <v>263</v>
       </c>
@@ -12161,7 +12165,7 @@
         <v>6.0650887573964495E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:13" ht="21">
       <c r="A244" s="24" t="s">
         <v>264</v>
       </c>
@@ -12203,7 +12207,7 @@
         <v>5.5145248645987195E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:13" ht="21">
       <c r="A245" s="24" t="s">
         <v>265</v>
       </c>
@@ -12245,7 +12249,7 @@
         <v>5.2901289895171656E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:13" ht="21">
       <c r="A246" s="24" t="s">
         <v>266</v>
       </c>
@@ -12287,7 +12291,7 @@
         <v>5.1135431444647113E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:13" ht="21">
       <c r="A247" s="24" t="s">
         <v>267</v>
       </c>
@@ -12329,7 +12333,7 @@
         <v>5.0238075829429338E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:13" ht="21">
       <c r="A248" s="24" t="s">
         <v>268</v>
       </c>
@@ -12371,7 +12375,7 @@
         <v>4.8310435337794701E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:13" ht="21">
       <c r="A249" s="24" t="s">
         <v>269</v>
       </c>
@@ -12413,7 +12417,7 @@
         <v>4.8002323750983844E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:13" ht="21">
       <c r="A250" s="24" t="s">
         <v>270</v>
       </c>
@@ -12455,7 +12459,7 @@
         <v>4.6311326524512218E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:13" ht="21">
       <c r="A251" s="24" t="s">
         <v>271</v>
       </c>
@@ -12497,7 +12501,7 @@
         <v>4.5235451874797258E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:13" ht="21">
       <c r="A252" s="24" t="s">
         <v>272</v>
       </c>
@@ -12539,7 +12543,7 @@
         <v>4.6859478329974745E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:13" ht="21">
       <c r="A253" s="24" t="s">
         <v>273</v>
       </c>
@@ -12581,7 +12585,7 @@
         <v>4.6457563707381348E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:13" ht="21">
       <c r="A254" s="24" t="s">
         <v>274</v>
       </c>
@@ -12623,7 +12627,7 @@
         <v>4.530471623446157E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:13" ht="21">
       <c r="A255" s="24" t="s">
         <v>275</v>
       </c>
@@ -12665,7 +12669,7 @@
         <v>4.3856926448038326E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:13" ht="21">
       <c r="A256" s="24" t="s">
         <v>276</v>
       </c>
@@ -12707,7 +12711,7 @@
         <v>4.3354635674750515E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:13" ht="21">
       <c r="A257" s="24" t="s">
         <v>277</v>
       </c>
@@ -12749,7 +12753,7 @@
         <v>4.3946943451436141E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:13" ht="21">
       <c r="A258" s="24" t="s">
         <v>278</v>
       </c>
@@ -12791,7 +12795,7 @@
         <v>4.3379573570780712E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:13" ht="21">
       <c r="A259" s="24" t="s">
         <v>279</v>
       </c>
@@ -12833,7 +12837,7 @@
         <v>4.278547703584927E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:13" ht="21">
       <c r="A260" s="24" t="s">
         <v>280</v>
       </c>
@@ -12875,7 +12879,7 @@
         <v>4.1873798033310344E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:13" ht="21">
       <c r="A261" s="24" t="s">
         <v>281</v>
       </c>
@@ -12917,7 +12921,7 @@
         <v>4.1229163490939087E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:13" ht="21">
       <c r="A262" s="24" t="s">
         <v>282</v>
       </c>
@@ -12959,7 +12963,7 @@
         <v>4.0203553285944327E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:13" ht="21">
       <c r="A263" s="24" t="s">
         <v>283</v>
       </c>
@@ -13001,7 +13005,7 @@
         <v>3.9329735168603296E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:13" ht="21">
       <c r="A264" s="24" t="s">
         <v>284</v>
       </c>
@@ -13043,7 +13047,7 @@
         <v>3.8807691122817671E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:13" ht="21">
       <c r="A265" s="24" t="s">
         <v>285</v>
       </c>
@@ -13085,7 +13089,7 @@
         <v>3.8731332520421144E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:13" ht="21">
       <c r="A266" s="24" t="s">
         <v>286</v>
       </c>
@@ -13127,7 +13131,7 @@
         <v>3.8674274912044247E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:13" ht="21">
       <c r="A267" s="24" t="s">
         <v>287</v>
       </c>
@@ -13169,7 +13173,7 @@
         <v>3.7261649676427942E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:13" ht="21">
       <c r="A268" s="24" t="s">
         <v>288</v>
       </c>
@@ -13211,7 +13215,7 @@
         <v>3.6882463098075004E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:13" ht="21">
       <c r="A269" s="24" t="s">
         <v>289</v>
       </c>
@@ -13253,7 +13257,7 @@
         <v>3.7361331731948909E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:13" ht="21">
       <c r="A270" s="24" t="s">
         <v>290</v>
       </c>
@@ -13295,7 +13299,7 @@
         <v>3.6729582483410364E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:13" ht="21">
       <c r="A271" s="24" t="s">
         <v>291</v>
       </c>
@@ -13337,7 +13341,7 @@
         <v>3.6206512806464863E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:13" ht="21">
       <c r="A272" s="24" t="s">
         <v>292</v>
       </c>
@@ -13379,7 +13383,7 @@
         <v>3.5752780937530614E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:13" ht="21">
       <c r="A273" s="24" t="s">
         <v>293</v>
       </c>
@@ -13421,7 +13425,7 @@
         <v>3.5689767690208409E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:13" ht="21">
       <c r="A274" s="24" t="s">
         <v>294</v>
       </c>
@@ -13463,7 +13467,7 @@
         <v>3.5426044914335375E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:13" ht="21">
       <c r="A275" s="24" t="s">
         <v>295</v>
       </c>
@@ -13505,7 +13509,7 @@
         <v>3.4928374725246965E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:13" ht="21">
       <c r="A276" s="24" t="s">
         <v>296</v>
       </c>
@@ -13547,7 +13551,7 @@
         <v>3.4626941470227268E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:13" ht="21">
       <c r="A277" s="24" t="s">
         <v>297</v>
       </c>
@@ -13589,7 +13593,7 @@
         <v>3.4734669836305923E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:13" ht="21">
       <c r="A278" s="24" t="s">
         <v>298</v>
       </c>
@@ -13631,7 +13635,7 @@
         <v>3.4062143299398953E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:13" ht="21">
       <c r="A279" s="24" t="s">
         <v>299</v>
       </c>
@@ -13673,7 +13677,7 @@
         <v>3.3389902596992427E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:13" ht="21">
       <c r="A280" s="24" t="s">
         <v>300</v>
       </c>
@@ -13715,7 +13719,7 @@
         <v>3.319795161575137E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:13" ht="21">
       <c r="A281" s="24" t="s">
         <v>301</v>
       </c>
@@ -13757,7 +13761,7 @@
         <v>3.3262208183872509E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:13" ht="21">
       <c r="A282" s="24" t="s">
         <v>302</v>
       </c>
@@ -13799,7 +13803,7 @@
         <v>3.2571442866553814E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:13" ht="21">
       <c r="A283" s="24" t="s">
         <v>303</v>
       </c>
@@ -13841,7 +13845,7 @@
         <v>3.2131980116677589E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:13" ht="21">
       <c r="A284" s="24" t="s">
         <v>304</v>
       </c>
@@ -13883,7 +13887,7 @@
         <v>3.168177381692687E-2</v>
       </c>
     </row>
-    <row r="285" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:13" ht="21">
       <c r="A285" s="24" t="s">
         <v>305</v>
       </c>
@@ -13925,7 +13929,7 @@
         <v>3.1449998358987825E-2</v>
       </c>
     </row>
-    <row r="286" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:13" ht="21">
       <c r="A286" s="24" t="s">
         <v>306</v>
       </c>
@@ -13967,7 +13971,7 @@
         <v>3.1457401862258504E-2</v>
       </c>
     </row>
-    <row r="287" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:13" ht="18.75">
       <c r="A287" s="22"/>
       <c r="B287" s="22"/>
       <c r="C287" s="22"/>
@@ -13989,7 +13993,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
saving pics with relative prices and use also in the main_file read_data2
</commit_message>
<xml_diff>
--- a/Data/dataset_main.xlsx
+++ b/Data/dataset_main.xlsx
@@ -1962,10 +1962,10 @@
   <dimension ref="A1:M288"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.3125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2052,7 +2052,7 @@
         <v>3</v>
       </c>
       <c r="M2" s="22">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.65">
@@ -2090,10 +2090,10 @@
         <v>0</v>
       </c>
       <c r="L3" s="21">
+        <v>1</v>
+      </c>
+      <c r="M3" s="22">
         <v>0</v>
-      </c>
-      <c r="M3" s="22">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="21" x14ac:dyDescent="0.65">
@@ -2161,7 +2161,9 @@
       <c r="I5" s="22"/>
       <c r="J5" s="21"/>
       <c r="K5" s="22"/>
-      <c r="L5" s="21"/>
+      <c r="L5" s="21">
+        <v>6</v>
+      </c>
       <c r="M5" s="22">
         <v>6</v>
       </c>

</xml_diff>